<commit_message>
doc: add light parallel mode test results
</commit_message>
<xml_diff>
--- a/.docs/performance_test.xlsx
+++ b/.docs/performance_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-project\github\setrem-parallel-programming\.docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA29DEE-8083-47A5-977F-BF7389A32B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7391FC0A-8EE2-4E83-8517-30169C29A703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sequential" sheetId="1" state="hidden" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="27">
   <si>
     <t>VM com 5 vCores</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Number of workers</t>
   </si>
   <si>
-    <t>Troughput</t>
-  </si>
-  <si>
     <t>Eixo X</t>
   </si>
   <si>
@@ -114,6 +111,15 @@
   </si>
   <si>
     <t>Parallel test (same machine - light way ON)</t>
+  </si>
+  <si>
+    <t>Complete parallel mode</t>
+  </si>
+  <si>
+    <t>Light parallel mode</t>
+  </si>
+  <si>
+    <t>The</t>
   </si>
 </sst>
 </file>
@@ -239,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,11 +322,7 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,6 +369,7 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,7 +773,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Troughput</c:v>
+                  <c:v>Throughput</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -831,7 +834,7 @@
                   <c:v>4649.4029294504235</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5434.9836444001312</c:v>
+                  <c:v>5778.0613592740383</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -985,6 +988,1646 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metrics!$D$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speedup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>metrics!$D$29:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.2773538825599564</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2949191030371843</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2276478991406088</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2257-40EE-8BA5-7E33ECD998C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="584146944"/>
+        <c:axId val="487906240"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="584146944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="487906240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="487906240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="584146944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metrics!$E$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Throughput</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>metrics!$E$29:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5279.7587380201294</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8567.6938237220256</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8595.885659030946</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5A13-457B-8CD4-50C9DB5AA622}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="657161200"/>
+        <c:axId val="657161680"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="657161200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="657161680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="657161680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="657161200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -1054,6 +2697,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E871A76-A8A2-3B24-715F-10ADD3A17E4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3B2F150-29B2-4D12-815D-0642D182392B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2329,8 +4044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:AF47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView topLeftCell="K19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE48" sqref="AE48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,7 +4664,7 @@
       <c r="AA9" s="29">
         <v>3</v>
       </c>
-      <c r="AB9" s="29">
+      <c r="AB9" s="53">
         <v>9.3026</v>
       </c>
       <c r="AC9" s="32">
@@ -2966,7 +4681,7 @@
       </c>
       <c r="AF9" s="3">
         <f>AVERAGE(AC9:AC13)</f>
-        <v>4323.7567973357154</v>
+        <v>5352.989941957434</v>
       </c>
     </row>
     <row r="10" spans="2:32" x14ac:dyDescent="0.25">
@@ -3029,7 +4744,7 @@
       <c r="AA10" s="29">
         <v>3</v>
       </c>
-      <c r="AB10" s="29">
+      <c r="AB10" s="53">
         <v>9.2286999999999999</v>
       </c>
       <c r="AC10" s="32">
@@ -3100,11 +4815,11 @@
       <c r="AA11" s="29">
         <v>3</v>
       </c>
-      <c r="AB11" s="29">
+      <c r="AB11" s="53">
         <v>8.2744</v>
       </c>
       <c r="AC11" s="32">
-        <f>Z11/AB11</f>
+        <f t="shared" ref="AC11:AC13" si="0">Z11/AB11</f>
         <v>6042.7342163782268</v>
       </c>
       <c r="AD11" s="2"/>
@@ -3171,11 +4886,11 @@
       <c r="AA12" s="29">
         <v>3</v>
       </c>
-      <c r="AB12" s="29">
+      <c r="AB12" s="53">
         <v>10.4541</v>
       </c>
       <c r="AC12" s="32">
-        <f>Z12/AB12</f>
+        <f t="shared" si="0"/>
         <v>4782.8124850537106</v>
       </c>
       <c r="AD12" s="2"/>
@@ -3242,12 +4957,12 @@
       <c r="AA13" s="29">
         <v>3</v>
       </c>
-      <c r="AB13" s="34">
-        <v>97150</v>
+      <c r="AB13" s="53">
+        <v>9.7149999999999999</v>
       </c>
       <c r="AC13" s="32">
-        <f>Z13/AB13</f>
-        <v>0.51466803911477099</v>
+        <f t="shared" si="0"/>
+        <v>5146.68039114771</v>
       </c>
       <c r="AD13" s="2"/>
       <c r="AE13" s="3"/>
@@ -3259,27 +4974,27 @@
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
       <c r="K14" s="31"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
       <c r="S14" s="17"/>
       <c r="T14" s="31"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="34"/>
+      <c r="W14" s="34"/>
       <c r="X14" s="17"/>
       <c r="Y14" s="17"/>
       <c r="Z14" s="17"/>
       <c r="AA14" s="17"/>
       <c r="AB14" s="17"/>
       <c r="AC14" s="31"/>
-      <c r="AD14" s="35"/>
-      <c r="AE14" s="35"/>
-      <c r="AF14" s="35"/>
+      <c r="AD14" s="34"/>
+      <c r="AE14" s="34"/>
+      <c r="AF14" s="34"/>
     </row>
     <row r="15" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B15" s="27">
@@ -3666,249 +5381,337 @@
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
     </row>
-    <row r="20" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="36"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="29"/>
-      <c r="S20" s="29"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="33"/>
-      <c r="V20" s="33"/>
-      <c r="W20" s="33"/>
-      <c r="X20" s="17"/>
-      <c r="Y20" s="29"/>
-      <c r="Z20" s="29"/>
-      <c r="AA20" s="29"/>
-      <c r="AB20" s="29"/>
-      <c r="AC20" s="32"/>
-      <c r="AD20" s="33"/>
-      <c r="AE20" s="33"/>
-      <c r="AF20" s="33"/>
-    </row>
-    <row r="21" spans="2:32" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="15"/>
-      <c r="E21" s="37"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="41">
+    <row r="20" spans="2:32" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="15"/>
+      <c r="E20" s="35"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="39">
         <f>MEDIAN(M3,M9,M15)</f>
         <v>0.76684661340243288</v>
       </c>
-      <c r="N21" s="41">
+      <c r="N20" s="39">
         <f>AVERAGE(N3,N9,N15)</f>
         <v>2801.2535394421488</v>
       </c>
-      <c r="O21" s="41"/>
-      <c r="P21" s="41"/>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="41"/>
-      <c r="S21" s="41"/>
-      <c r="T21" s="39"/>
-      <c r="U21" s="41"/>
-      <c r="V21" s="41">
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="39"/>
+      <c r="S20" s="39"/>
+      <c r="T20" s="37"/>
+      <c r="U20" s="39"/>
+      <c r="V20" s="39">
         <f>MEDIAN(V3,V9,V15)</f>
         <v>1.2350227209496429</v>
       </c>
-      <c r="W21" s="41">
+      <c r="W20" s="39">
         <f>AVERAGE(W3,W9,W15)</f>
         <v>4649.4029294504235</v>
       </c>
-      <c r="X21" s="41"/>
-      <c r="Y21" s="41"/>
-      <c r="Z21" s="41"/>
-      <c r="AA21" s="41"/>
-      <c r="AB21" s="41"/>
-      <c r="AC21" s="39"/>
-      <c r="AD21" s="41"/>
-      <c r="AE21" s="41">
+      <c r="X20" s="39"/>
+      <c r="Y20" s="39"/>
+      <c r="Z20" s="39"/>
+      <c r="AA20" s="39"/>
+      <c r="AB20" s="39"/>
+      <c r="AC20" s="37"/>
+      <c r="AD20" s="39"/>
+      <c r="AE20" s="39">
         <f>MEDIAN(AE3,AE9,AE15)</f>
         <v>1.5533490799871694</v>
       </c>
-      <c r="AF21" s="41">
+      <c r="AF20" s="39">
         <f>AVERAGE(AF3,AF9,AF15)</f>
-        <v>5434.9836444001312</v>
-      </c>
+        <v>5778.0613592740383</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="D21" s="13"/>
+      <c r="E21" s="16"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="31"/>
+      <c r="U21" s="34"/>
+      <c r="V21" s="34"/>
+      <c r="W21" s="34"/>
+      <c r="X21" s="17"/>
+      <c r="Y21" s="17"/>
+      <c r="Z21" s="17"/>
+      <c r="AA21" s="17"/>
+      <c r="AB21" s="17"/>
+      <c r="AC21" s="31"/>
+      <c r="AD21" s="34"/>
+      <c r="AE21" s="34"/>
+      <c r="AF21" s="34"/>
     </row>
     <row r="22" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D22" s="13"/>
-      <c r="E22" s="16"/>
       <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
+      <c r="H22" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="I22" s="17"/>
-      <c r="J22" s="38"/>
+      <c r="J22" s="17"/>
       <c r="K22" s="31"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="35"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="17"/>
       <c r="R22" s="17"/>
       <c r="S22" s="17"/>
       <c r="T22" s="31"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
+      <c r="U22" s="34"/>
+      <c r="V22" s="34"/>
+      <c r="W22" s="34"/>
       <c r="X22" s="17"/>
       <c r="Y22" s="17"/>
       <c r="Z22" s="17"/>
       <c r="AA22" s="17"/>
       <c r="AB22" s="17"/>
       <c r="AC22" s="31"/>
-      <c r="AD22" s="35"/>
-      <c r="AE22" s="35"/>
-      <c r="AF22" s="35"/>
+      <c r="AD22" s="34"/>
+      <c r="AE22" s="34"/>
+      <c r="AF22" s="34"/>
     </row>
     <row r="23" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="D23" s="13"/>
       <c r="G23" s="17"/>
       <c r="H23" s="17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
       <c r="K23" s="31"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
       <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="31"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="35"/>
       <c r="X23" s="17"/>
       <c r="Y23" s="17"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="17"/>
       <c r="AB23" s="17"/>
       <c r="AC23" s="31"/>
-      <c r="AD23" s="35"/>
-      <c r="AE23" s="35"/>
-      <c r="AF23" s="35"/>
+      <c r="AD23" s="34"/>
+      <c r="AE23" s="34"/>
+      <c r="AF23" s="34"/>
     </row>
     <row r="24" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="G24" s="17"/>
-      <c r="H24" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="17"/>
-      <c r="X24" s="17"/>
-      <c r="Y24" s="17"/>
-      <c r="Z24" s="17"/>
-      <c r="AA24" s="17"/>
-      <c r="AB24" s="17"/>
-      <c r="AC24" s="31"/>
-      <c r="AD24" s="35"/>
-      <c r="AE24" s="35"/>
-      <c r="AF24" s="35"/>
-    </row>
-    <row r="25" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="H25" t="s">
+      <c r="H24" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="G27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="23"/>
+      <c r="P27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="21"/>
+      <c r="W27" s="23"/>
+      <c r="Y27" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7"/>
+      <c r="AC27" s="7"/>
+      <c r="AD27" s="7"/>
+      <c r="AE27" s="23"/>
+      <c r="AF27" s="23"/>
+    </row>
     <row r="28" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="G28" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="23"/>
-      <c r="P28" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="21"/>
-      <c r="W28" s="23"/>
+      <c r="G28" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="L28" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="M28" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="N28" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="P28" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q28" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="R28" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="S28" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="T28" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="U28" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="V28" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="W28" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y28" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z28" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA28" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB28" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC28" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD28" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE28" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF28" s="24" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="29" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="G29" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H29" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="J29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K29" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="L29" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="M29" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="N29" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="P29" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q29" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="R29" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="S29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T29" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="U29" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="V29" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="W29" s="24" t="s">
-        <v>14</v>
+      <c r="G29" s="27">
+        <v>1</v>
+      </c>
+      <c r="H29" s="27">
+        <v>30000</v>
+      </c>
+      <c r="I29" s="27">
+        <v>1</v>
+      </c>
+      <c r="J29" s="29">
+        <v>3.5956999999999999</v>
+      </c>
+      <c r="K29" s="30">
+        <f>H29/J29</f>
+        <v>8343.298940401035</v>
+      </c>
+      <c r="L29" s="41">
+        <f>MEDIAN(J29:J33)</f>
+        <v>3.2879999999999998</v>
+      </c>
+      <c r="M29" s="44">
+        <f>E3/L29</f>
+        <v>1.6201034063260342</v>
+      </c>
+      <c r="N29" s="44">
+        <f>AVERAGE(K29:K33)</f>
+        <v>8916.4115942682383</v>
+      </c>
+      <c r="P29" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="27">
+        <v>30000</v>
+      </c>
+      <c r="R29" s="27">
+        <v>2</v>
+      </c>
+      <c r="S29" s="29">
+        <v>2.1880999999999999</v>
+      </c>
+      <c r="T29" s="30">
+        <f>Q29/S29</f>
+        <v>13710.525113111833</v>
+      </c>
+      <c r="U29" s="41">
+        <f>MEDIAN(S29:S33)</f>
+        <v>2.1825999999999999</v>
+      </c>
+      <c r="V29" s="44">
+        <f>E3/U29</f>
+        <v>2.4406212773756075</v>
+      </c>
+      <c r="W29" s="44">
+        <f>AVERAGE(T29:T33)</f>
+        <v>13663.669578564508</v>
+      </c>
+      <c r="Y29" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="27">
+        <v>30000</v>
+      </c>
+      <c r="AA29" s="27">
+        <v>3</v>
+      </c>
+      <c r="AB29" s="29">
+        <v>2.1032000000000002</v>
+      </c>
+      <c r="AC29" s="30">
+        <f>Z29/AB29</f>
+        <v>14263.978699125142</v>
+      </c>
+      <c r="AD29" s="4">
+        <f>MEDIAN(AB29:AB33)</f>
+        <v>2.1032000000000002</v>
+      </c>
+      <c r="AE29" s="5">
+        <f>E3/AD29</f>
+        <v>2.5327596044123242</v>
+      </c>
+      <c r="AF29" s="5">
+        <f>AVERAGE(AC29:AC33)</f>
+        <v>14487.501618863946</v>
       </c>
     </row>
     <row r="30" spans="2:32" x14ac:dyDescent="0.25">
       <c r="G30" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="27">
         <v>30000</v>
@@ -3917,26 +5720,17 @@
         <v>1</v>
       </c>
       <c r="J30" s="29">
-        <v>3.5956999999999999</v>
+        <v>3.2065000000000001</v>
       </c>
       <c r="K30" s="30">
         <f>H30/J30</f>
-        <v>8343.298940401035</v>
-      </c>
-      <c r="L30" s="43">
-        <f>MEDIAN(J30:J34)</f>
-        <v>3.2879999999999998</v>
-      </c>
-      <c r="M30" s="46">
-        <f>E3/L30</f>
-        <v>1.6201034063260342</v>
-      </c>
-      <c r="N30" s="46">
-        <f>AVERAGE(K30:K34)</f>
-        <v>8916.4115942682383</v>
-      </c>
+        <v>9355.9956338687043</v>
+      </c>
+      <c r="L30" s="42"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
       <c r="P30" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q30" s="27">
         <v>30000</v>
@@ -3945,28 +5739,38 @@
         <v>2</v>
       </c>
       <c r="S30" s="29">
-        <v>2.1880999999999999</v>
+        <v>2.1825999999999999</v>
       </c>
       <c r="T30" s="30">
         <f>Q30/S30</f>
-        <v>13710.525113111833</v>
-      </c>
-      <c r="U30" s="43">
-        <f>MEDIAN(S30:S34)</f>
-        <v>2.1825999999999999</v>
-      </c>
-      <c r="V30" s="46">
-        <f>E3/U30</f>
-        <v>2.4406212773756075</v>
-      </c>
-      <c r="W30" s="46">
-        <f>AVERAGE(T30:T34)</f>
-        <v>13663.669578564508</v>
-      </c>
+        <v>13745.074681572438</v>
+      </c>
+      <c r="U30" s="42"/>
+      <c r="V30" s="45"/>
+      <c r="W30" s="45"/>
+      <c r="Y30" s="27">
+        <v>2</v>
+      </c>
+      <c r="Z30" s="27">
+        <v>30000</v>
+      </c>
+      <c r="AA30" s="27">
+        <v>3</v>
+      </c>
+      <c r="AB30" s="29">
+        <v>2.9695999999999998</v>
+      </c>
+      <c r="AC30" s="30">
+        <f>Z30/AB30</f>
+        <v>10102.370689655174</v>
+      </c>
+      <c r="AD30" s="4"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="5"/>
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.25">
       <c r="G31" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H31" s="27">
         <v>30000</v>
@@ -3975,17 +5779,17 @@
         <v>1</v>
       </c>
       <c r="J31" s="29">
-        <v>3.2065000000000001</v>
+        <v>3.5537000000000001</v>
       </c>
       <c r="K31" s="30">
         <f>H31/J31</f>
-        <v>9355.9956338687043</v>
-      </c>
-      <c r="L31" s="44"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="47"/>
+        <v>8441.9056194951736</v>
+      </c>
+      <c r="L31" s="42"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="45"/>
       <c r="P31" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q31" s="27">
         <v>30000</v>
@@ -3994,19 +5798,38 @@
         <v>2</v>
       </c>
       <c r="S31" s="29">
-        <v>2.1825999999999999</v>
+        <v>1.9893000000000001</v>
       </c>
       <c r="T31" s="30">
         <f>Q31/S31</f>
-        <v>13745.074681572438</v>
-      </c>
-      <c r="U31" s="44"/>
-      <c r="V31" s="47"/>
-      <c r="W31" s="47"/>
+        <v>15080.681646810435</v>
+      </c>
+      <c r="U31" s="42"/>
+      <c r="V31" s="45"/>
+      <c r="W31" s="45"/>
+      <c r="Y31" s="27">
+        <v>3</v>
+      </c>
+      <c r="Z31" s="27">
+        <v>30000</v>
+      </c>
+      <c r="AA31" s="27">
+        <v>3</v>
+      </c>
+      <c r="AB31" s="29">
+        <v>1.7062999999999999</v>
+      </c>
+      <c r="AC31" s="30">
+        <f>Z31/AB31</f>
+        <v>17581.902361835553</v>
+      </c>
+      <c r="AD31" s="4"/>
+      <c r="AE31" s="5"/>
+      <c r="AF31" s="5"/>
     </row>
     <row r="32" spans="2:32" x14ac:dyDescent="0.25">
       <c r="G32" s="27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H32" s="27">
         <v>30000</v>
@@ -4015,17 +5838,17 @@
         <v>1</v>
       </c>
       <c r="J32" s="29">
-        <v>3.5537000000000001</v>
+        <v>3.22</v>
       </c>
       <c r="K32" s="30">
         <f>H32/J32</f>
-        <v>8441.9056194951736</v>
-      </c>
-      <c r="L32" s="44"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
+        <v>9316.7701863354032</v>
+      </c>
+      <c r="L32" s="42"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="45"/>
       <c r="P32" s="27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q32" s="27">
         <v>30000</v>
@@ -4034,19 +5857,38 @@
         <v>2</v>
       </c>
       <c r="S32" s="29">
-        <v>1.9893000000000001</v>
+        <v>2.5629</v>
       </c>
       <c r="T32" s="30">
         <f>Q32/S32</f>
-        <v>15080.681646810435</v>
-      </c>
-      <c r="U32" s="44"/>
-      <c r="V32" s="47"/>
-      <c r="W32" s="47"/>
-    </row>
-    <row r="33" spans="7:23" x14ac:dyDescent="0.25">
+        <v>11705.489874751258</v>
+      </c>
+      <c r="U32" s="42"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="45"/>
+      <c r="Y32" s="27">
+        <v>4</v>
+      </c>
+      <c r="Z32" s="27">
+        <v>30000</v>
+      </c>
+      <c r="AA32" s="27">
+        <v>3</v>
+      </c>
+      <c r="AB32" s="29">
+        <v>2.1196999999999999</v>
+      </c>
+      <c r="AC32" s="30">
+        <f>Z32/AB32</f>
+        <v>14152.94617162806</v>
+      </c>
+      <c r="AD32" s="4"/>
+      <c r="AE32" s="5"/>
+      <c r="AF32" s="5"/>
+    </row>
+    <row r="33" spans="7:32" x14ac:dyDescent="0.25">
       <c r="G33" s="27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H33" s="27">
         <v>30000</v>
@@ -4055,17 +5897,17 @@
         <v>1</v>
       </c>
       <c r="J33" s="29">
-        <v>3.22</v>
+        <v>3.2879999999999998</v>
       </c>
       <c r="K33" s="30">
         <f>H33/J33</f>
-        <v>9316.7701863354032</v>
-      </c>
-      <c r="L33" s="44"/>
-      <c r="M33" s="47"/>
-      <c r="N33" s="47"/>
+        <v>9124.0875912408756</v>
+      </c>
+      <c r="L33" s="43"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
       <c r="P33" s="27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q33" s="27">
         <v>30000</v>
@@ -4074,63 +5916,129 @@
         <v>2</v>
       </c>
       <c r="S33" s="29">
-        <v>2.5629</v>
+        <v>2.1312000000000002</v>
       </c>
       <c r="T33" s="30">
         <f>Q33/S33</f>
-        <v>11705.489874751258</v>
-      </c>
-      <c r="U33" s="44"/>
-      <c r="V33" s="47"/>
-      <c r="W33" s="47"/>
-    </row>
-    <row r="34" spans="7:23" x14ac:dyDescent="0.25">
-      <c r="G34" s="27">
+        <v>14076.576576576575</v>
+      </c>
+      <c r="U33" s="43"/>
+      <c r="V33" s="46"/>
+      <c r="W33" s="46"/>
+      <c r="Y33" s="27">
         <v>5</v>
       </c>
-      <c r="H34" s="27">
+      <c r="Z33" s="27">
         <v>30000</v>
       </c>
-      <c r="I34" s="27">
-        <v>1</v>
-      </c>
-      <c r="J34" s="29">
-        <v>3.2879999999999998</v>
-      </c>
-      <c r="K34" s="30">
-        <f>H34/J34</f>
-        <v>9124.0875912408756</v>
-      </c>
-      <c r="L34" s="45"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="48"/>
-      <c r="P34" s="27">
-        <v>5</v>
-      </c>
-      <c r="Q34" s="27">
-        <v>30000</v>
-      </c>
-      <c r="R34" s="27">
-        <v>2</v>
-      </c>
-      <c r="S34" s="29">
-        <v>2.1312000000000002</v>
-      </c>
-      <c r="T34" s="30">
-        <f>Q34/S34</f>
-        <v>14076.576576576575</v>
-      </c>
-      <c r="U34" s="45"/>
-      <c r="V34" s="48"/>
-      <c r="W34" s="48"/>
-    </row>
-    <row r="35" spans="7:23" x14ac:dyDescent="0.25">
-      <c r="K35" s="31"/>
-      <c r="T35" s="31"/>
-    </row>
-    <row r="36" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="AA33" s="27">
+        <v>3</v>
+      </c>
+      <c r="AB33" s="29">
+        <v>1.8364</v>
+      </c>
+      <c r="AC33" s="30">
+        <f>Z33/AB33</f>
+        <v>16336.3101720758</v>
+      </c>
+      <c r="AD33" s="4"/>
+      <c r="AE33" s="5"/>
+      <c r="AF33" s="5"/>
+    </row>
+    <row r="34" spans="7:32" x14ac:dyDescent="0.25">
+      <c r="K34" s="31"/>
+      <c r="T34" s="31"/>
+      <c r="AC34" s="31"/>
+    </row>
+    <row r="35" spans="7:32" x14ac:dyDescent="0.25">
+      <c r="G35" s="29">
+        <v>1</v>
+      </c>
+      <c r="H35" s="29">
+        <v>50000</v>
+      </c>
+      <c r="I35" s="27">
+        <v>1</v>
+      </c>
+      <c r="J35" s="29">
+        <v>8.7312999999999992</v>
+      </c>
+      <c r="K35" s="32">
+        <f>H35/J35</f>
+        <v>5726.5241143930461</v>
+      </c>
+      <c r="L35" s="47">
+        <f>MEDIAN(J35:J39)</f>
+        <v>10.7982</v>
+      </c>
+      <c r="M35" s="50">
+        <f>E9/L35</f>
+        <v>1.2728510307273435</v>
+      </c>
+      <c r="N35" s="50">
+        <f>AVERAGE(K35:K39)</f>
+        <v>4826.0918702505669</v>
+      </c>
+      <c r="P35" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="29">
+        <v>50000</v>
+      </c>
+      <c r="R35" s="29">
+        <v>2</v>
+      </c>
+      <c r="S35" s="29">
+        <v>5.9890999999999996</v>
+      </c>
+      <c r="T35" s="32">
+        <f>Q35/S35</f>
+        <v>8348.4997745905057</v>
+      </c>
+      <c r="U35" s="47">
+        <f>MEDIAN(S35:S39)</f>
+        <v>5.9890999999999996</v>
+      </c>
+      <c r="V35" s="50">
+        <f>E9/U35</f>
+        <v>2.2949191030371843</v>
+      </c>
+      <c r="W35" s="50">
+        <f>AVERAGE(T35:T39)</f>
+        <v>8512.4818313888645</v>
+      </c>
+      <c r="Y35" s="29">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="29">
+        <v>50000</v>
+      </c>
+      <c r="AA35" s="29">
+        <v>3</v>
+      </c>
+      <c r="AB35" s="53">
+        <v>10.2765</v>
+      </c>
+      <c r="AC35" s="32">
+        <f>Z35/AB35</f>
+        <v>4865.4697611054344</v>
+      </c>
+      <c r="AD35" s="2">
+        <f>MEDIAN(AB35:AB39)</f>
+        <v>6.5446</v>
+      </c>
+      <c r="AE35" s="3">
+        <f>E9/AD35</f>
+        <v>2.1001283500901509</v>
+      </c>
+      <c r="AF35" s="3">
+        <f>AVERAGE(AC35:AC39)</f>
+        <v>7461.6203598259108</v>
+      </c>
+    </row>
+    <row r="36" spans="7:32" x14ac:dyDescent="0.25">
       <c r="G36" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H36" s="29">
         <v>50000</v>
@@ -4139,26 +6047,17 @@
         <v>1</v>
       </c>
       <c r="J36" s="29">
-        <v>8.7312999999999992</v>
+        <v>10.9229</v>
       </c>
       <c r="K36" s="32">
         <f>H36/J36</f>
-        <v>5726.5241143930461</v>
-      </c>
-      <c r="L36" s="49">
-        <f>MEDIAN(J36:J40)</f>
-        <v>10.7982</v>
-      </c>
-      <c r="M36" s="52">
-        <f>E9/L36</f>
-        <v>1.2728510307273435</v>
-      </c>
-      <c r="N36" s="52">
-        <f>AVERAGE(K36:K40)</f>
-        <v>4826.0918702505669</v>
-      </c>
+        <v>4577.5389319686165</v>
+      </c>
+      <c r="L36" s="48"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="51"/>
       <c r="P36" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q36" s="29">
         <v>50000</v>
@@ -4167,28 +6066,38 @@
         <v>2</v>
       </c>
       <c r="S36" s="29">
-        <v>5.9890999999999996</v>
+        <v>5.1974</v>
       </c>
       <c r="T36" s="32">
         <f>Q36/S36</f>
-        <v>8348.4997745905057</v>
-      </c>
-      <c r="U36" s="49">
-        <f>MEDIAN(S36:S40)</f>
-        <v>5.9890999999999996</v>
-      </c>
-      <c r="V36" s="52">
-        <f>E9/U36</f>
-        <v>2.2949191030371843</v>
-      </c>
-      <c r="W36" s="52">
-        <f>AVERAGE(T36:T40)</f>
-        <v>8512.4818313888645</v>
-      </c>
-    </row>
-    <row r="37" spans="7:23" x14ac:dyDescent="0.25">
+        <v>9620.1947127409858</v>
+      </c>
+      <c r="U36" s="48"/>
+      <c r="V36" s="51"/>
+      <c r="W36" s="51"/>
+      <c r="Y36" s="29">
+        <v>2</v>
+      </c>
+      <c r="Z36" s="29">
+        <v>50000</v>
+      </c>
+      <c r="AA36" s="29">
+        <v>3</v>
+      </c>
+      <c r="AB36" s="53">
+        <v>7.6410999999999998</v>
+      </c>
+      <c r="AC36" s="32">
+        <f>Z36/AB36</f>
+        <v>6543.5604821295365</v>
+      </c>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="3"/>
+    </row>
+    <row r="37" spans="7:32" x14ac:dyDescent="0.25">
       <c r="G37" s="29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H37" s="29">
         <v>50000</v>
@@ -4197,17 +6106,17 @@
         <v>1</v>
       </c>
       <c r="J37" s="29">
-        <v>10.9229</v>
+        <v>11.375500000000001</v>
       </c>
       <c r="K37" s="32">
         <f>H37/J37</f>
-        <v>4577.5389319686165</v>
-      </c>
-      <c r="L37" s="50"/>
-      <c r="M37" s="53"/>
-      <c r="N37" s="53"/>
+        <v>4395.4111907168917</v>
+      </c>
+      <c r="L37" s="48"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="51"/>
       <c r="P37" s="29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q37" s="29">
         <v>50000</v>
@@ -4216,19 +6125,38 @@
         <v>2</v>
       </c>
       <c r="S37" s="29">
-        <v>5.1974</v>
+        <v>5.8849</v>
       </c>
       <c r="T37" s="32">
         <f>Q37/S37</f>
-        <v>9620.1947127409858</v>
-      </c>
-      <c r="U37" s="50"/>
-      <c r="V37" s="53"/>
-      <c r="W37" s="53"/>
-    </row>
-    <row r="38" spans="7:23" x14ac:dyDescent="0.25">
+        <v>8496.3210929667457</v>
+      </c>
+      <c r="U37" s="48"/>
+      <c r="V37" s="51"/>
+      <c r="W37" s="51"/>
+      <c r="Y37" s="29">
+        <v>3</v>
+      </c>
+      <c r="Z37" s="29">
+        <v>50000</v>
+      </c>
+      <c r="AA37" s="29">
+        <v>3</v>
+      </c>
+      <c r="AB37" s="53">
+        <v>6.5446</v>
+      </c>
+      <c r="AC37" s="32">
+        <f>Z37/AB37</f>
+        <v>7639.8863184915808</v>
+      </c>
+      <c r="AD37" s="2"/>
+      <c r="AE37" s="3"/>
+      <c r="AF37" s="3"/>
+    </row>
+    <row r="38" spans="7:32" x14ac:dyDescent="0.25">
       <c r="G38" s="29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H38" s="29">
         <v>50000</v>
@@ -4237,17 +6165,17 @@
         <v>1</v>
       </c>
       <c r="J38" s="29">
-        <v>11.375500000000001</v>
+        <v>10.7982</v>
       </c>
       <c r="K38" s="32">
         <f>H38/J38</f>
-        <v>4395.4111907168917</v>
-      </c>
-      <c r="L38" s="50"/>
-      <c r="M38" s="53"/>
-      <c r="N38" s="53"/>
+        <v>4630.4013631901616</v>
+      </c>
+      <c r="L38" s="48"/>
+      <c r="M38" s="51"/>
+      <c r="N38" s="51"/>
       <c r="P38" s="29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q38" s="29">
         <v>50000</v>
@@ -4256,19 +6184,38 @@
         <v>2</v>
       </c>
       <c r="S38" s="29">
-        <v>5.8849</v>
+        <v>6.1283000000000003</v>
       </c>
       <c r="T38" s="32">
         <f>Q38/S38</f>
-        <v>8496.3210929667457</v>
-      </c>
-      <c r="U38" s="50"/>
-      <c r="V38" s="53"/>
-      <c r="W38" s="53"/>
-    </row>
-    <row r="39" spans="7:23" x14ac:dyDescent="0.25">
+        <v>8158.869507041104</v>
+      </c>
+      <c r="U38" s="48"/>
+      <c r="V38" s="51"/>
+      <c r="W38" s="51"/>
+      <c r="Y38" s="29">
+        <v>4</v>
+      </c>
+      <c r="Z38" s="29">
+        <v>50000</v>
+      </c>
+      <c r="AA38" s="29">
+        <v>3</v>
+      </c>
+      <c r="AB38" s="53">
+        <v>5.7717999999999998</v>
+      </c>
+      <c r="AC38" s="32">
+        <f>Z38/AB38</f>
+        <v>8662.8088291347594</v>
+      </c>
+      <c r="AD38" s="2"/>
+      <c r="AE38" s="3"/>
+      <c r="AF38" s="3"/>
+    </row>
+    <row r="39" spans="7:32" x14ac:dyDescent="0.25">
       <c r="G39" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H39" s="29">
         <v>50000</v>
@@ -4277,17 +6224,17 @@
         <v>1</v>
       </c>
       <c r="J39" s="29">
-        <v>10.7982</v>
+        <v>10.4154</v>
       </c>
       <c r="K39" s="32">
         <f>H39/J39</f>
-        <v>4630.4013631901616</v>
-      </c>
-      <c r="L39" s="50"/>
-      <c r="M39" s="53"/>
-      <c r="N39" s="53"/>
+        <v>4800.5837509841194</v>
+      </c>
+      <c r="L39" s="49"/>
+      <c r="M39" s="52"/>
+      <c r="N39" s="52"/>
       <c r="P39" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q39" s="29">
         <v>50000</v>
@@ -4296,77 +6243,150 @@
         <v>2</v>
       </c>
       <c r="S39" s="29">
-        <v>6.1283000000000003</v>
+        <v>6.2984</v>
       </c>
       <c r="T39" s="32">
         <f>Q39/S39</f>
-        <v>8158.869507041104</v>
-      </c>
-      <c r="U39" s="50"/>
-      <c r="V39" s="53"/>
-      <c r="W39" s="53"/>
-    </row>
-    <row r="40" spans="7:23" x14ac:dyDescent="0.25">
-      <c r="G40" s="29">
+        <v>7938.5240696049786</v>
+      </c>
+      <c r="U39" s="49"/>
+      <c r="V39" s="52"/>
+      <c r="W39" s="52"/>
+      <c r="Y39" s="29">
         <v>5</v>
       </c>
-      <c r="H40" s="29">
+      <c r="Z39" s="29">
         <v>50000</v>
       </c>
-      <c r="I40" s="27">
-        <v>1</v>
-      </c>
-      <c r="J40" s="29">
-        <v>10.4154</v>
-      </c>
-      <c r="K40" s="32">
-        <f>H40/J40</f>
-        <v>4800.5837509841194</v>
-      </c>
-      <c r="L40" s="51"/>
-      <c r="M40" s="54"/>
-      <c r="N40" s="54"/>
-      <c r="P40" s="29">
-        <v>5</v>
-      </c>
-      <c r="Q40" s="29">
-        <v>50000</v>
-      </c>
-      <c r="R40" s="29">
-        <v>2</v>
-      </c>
-      <c r="S40" s="29">
-        <v>6.2984</v>
-      </c>
-      <c r="T40" s="32">
-        <f>Q40/S40</f>
-        <v>7938.5240696049786</v>
-      </c>
-      <c r="U40" s="51"/>
-      <c r="V40" s="54"/>
-      <c r="W40" s="54"/>
-    </row>
-    <row r="41" spans="7:23" x14ac:dyDescent="0.25">
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="35"/>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="P41" s="17"/>
-      <c r="Q41" s="17"/>
-      <c r="R41" s="17"/>
-      <c r="S41" s="17"/>
-      <c r="T41" s="31"/>
-      <c r="U41" s="35"/>
-      <c r="V41" s="35"/>
-      <c r="W41" s="35"/>
-    </row>
-    <row r="42" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="AA39" s="29">
+        <v>3</v>
+      </c>
+      <c r="AB39" s="53">
+        <v>5.2103000000000002</v>
+      </c>
+      <c r="AC39" s="32">
+        <f>Z39/AB39</f>
+        <v>9596.3764082682374</v>
+      </c>
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="3"/>
+      <c r="AF39" s="3"/>
+    </row>
+    <row r="40" spans="7:32" x14ac:dyDescent="0.25">
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="34"/>
+      <c r="N40" s="34"/>
+      <c r="P40" s="17"/>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="17"/>
+      <c r="S40" s="17"/>
+      <c r="T40" s="31"/>
+      <c r="U40" s="34"/>
+      <c r="V40" s="34"/>
+      <c r="W40" s="34"/>
+      <c r="Y40" s="17"/>
+      <c r="Z40" s="17"/>
+      <c r="AA40" s="17"/>
+      <c r="AB40" s="17"/>
+      <c r="AC40" s="31"/>
+      <c r="AD40" s="34"/>
+      <c r="AE40" s="34"/>
+      <c r="AF40" s="34"/>
+    </row>
+    <row r="41" spans="7:32" x14ac:dyDescent="0.25">
+      <c r="G41" s="29">
+        <v>1</v>
+      </c>
+      <c r="H41" s="29">
+        <v>100000</v>
+      </c>
+      <c r="I41" s="27">
+        <v>1</v>
+      </c>
+      <c r="J41" s="29">
+        <v>44.493099999999998</v>
+      </c>
+      <c r="K41" s="32">
+        <f>H41/J41</f>
+        <v>2247.539506125669</v>
+      </c>
+      <c r="L41" s="47">
+        <f>MEDIAN(J41:J45)</f>
+        <v>46.146099999999997</v>
+      </c>
+      <c r="M41" s="47">
+        <f>E15/L41</f>
+        <v>1.2773538825599564</v>
+      </c>
+      <c r="N41" s="47">
+        <f>AVERAGE(K41:K45)</f>
+        <v>2096.772749541582</v>
+      </c>
+      <c r="P41" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="29">
+        <v>100000</v>
+      </c>
+      <c r="R41" s="29">
+        <v>2</v>
+      </c>
+      <c r="S41" s="29">
+        <v>26.781199999999998</v>
+      </c>
+      <c r="T41" s="32">
+        <f>Q41/S41</f>
+        <v>3733.9626305019942</v>
+      </c>
+      <c r="U41" s="47">
+        <f>MEDIAN(S41:S45)</f>
+        <v>26.781199999999998</v>
+      </c>
+      <c r="V41" s="47">
+        <f>E15/U41</f>
+        <v>2.2009805385867698</v>
+      </c>
+      <c r="W41" s="47">
+        <f>AVERAGE(T41:T45)</f>
+        <v>3526.9300612127031</v>
+      </c>
+      <c r="Y41" s="29">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="29">
+        <v>100000</v>
+      </c>
+      <c r="AA41" s="29">
+        <v>3</v>
+      </c>
+      <c r="AB41" s="29">
+        <v>27.3447</v>
+      </c>
+      <c r="AC41" s="32">
+        <f>Z41/AB41</f>
+        <v>3657.0158019652804</v>
+      </c>
+      <c r="AD41" s="2">
+        <f>MEDIAN(AB41:AB45)</f>
+        <v>26.460599999999999</v>
+      </c>
+      <c r="AE41" s="2">
+        <f>E15/AD41</f>
+        <v>2.2276478991406088</v>
+      </c>
+      <c r="AF41" s="2">
+        <f>AVERAGE(AC41:AC45)</f>
+        <v>3838.534998402979</v>
+      </c>
+    </row>
+    <row r="42" spans="7:32" x14ac:dyDescent="0.25">
       <c r="G42" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H42" s="29">
         <v>100000</v>
@@ -4375,26 +6395,17 @@
         <v>1</v>
       </c>
       <c r="J42" s="29">
-        <v>44.493099999999998</v>
+        <v>46.146099999999997</v>
       </c>
       <c r="K42" s="32">
         <f>H42/J42</f>
-        <v>2247.539506125669</v>
-      </c>
-      <c r="L42" s="49">
-        <f>MEDIAN(J42:J46)</f>
-        <v>44.493099999999998</v>
-      </c>
-      <c r="M42" s="49">
-        <f>E15/L42</f>
-        <v>1.3248099143462695</v>
-      </c>
-      <c r="N42" s="49" t="e">
-        <f>AVERAGE(K42:K46)</f>
-        <v>#DIV/0!</v>
-      </c>
+        <v>2167.0303665965271</v>
+      </c>
+      <c r="L42" s="48"/>
+      <c r="M42" s="48"/>
+      <c r="N42" s="48"/>
       <c r="P42" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q42" s="29">
         <v>100000</v>
@@ -4403,28 +6414,38 @@
         <v>2</v>
       </c>
       <c r="S42" s="29">
-        <v>26.781199999999998</v>
+        <v>34.976300000000002</v>
       </c>
       <c r="T42" s="32">
         <f>Q42/S42</f>
-        <v>3733.9626305019942</v>
-      </c>
-      <c r="U42" s="49">
-        <f>MEDIAN(S42:S46)</f>
-        <v>26.781199999999998</v>
-      </c>
-      <c r="V42" s="49">
-        <f>E15/U42</f>
-        <v>2.2009805385867698</v>
-      </c>
-      <c r="W42" s="49">
-        <f>AVERAGE(T42:T46)</f>
-        <v>3526.9300612127031</v>
-      </c>
-    </row>
-    <row r="43" spans="7:23" x14ac:dyDescent="0.25">
+        <v>2859.0788619722498</v>
+      </c>
+      <c r="U42" s="48"/>
+      <c r="V42" s="48"/>
+      <c r="W42" s="48"/>
+      <c r="Y42" s="29">
+        <v>2</v>
+      </c>
+      <c r="Z42" s="29">
+        <v>100000</v>
+      </c>
+      <c r="AA42" s="29">
+        <v>3</v>
+      </c>
+      <c r="AB42" s="29">
+        <v>24.2742</v>
+      </c>
+      <c r="AC42" s="32">
+        <f>Z42/AB42</f>
+        <v>4119.6002339932929</v>
+      </c>
+      <c r="AD42" s="2"/>
+      <c r="AE42" s="2"/>
+      <c r="AF42" s="2"/>
+    </row>
+    <row r="43" spans="7:32" x14ac:dyDescent="0.25">
       <c r="G43" s="29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H43" s="29">
         <v>100000</v>
@@ -4432,16 +6453,18 @@
       <c r="I43" s="27">
         <v>1</v>
       </c>
-      <c r="J43" s="29"/>
-      <c r="K43" s="32" t="e">
+      <c r="J43" s="29">
+        <v>51.191099999999999</v>
+      </c>
+      <c r="K43" s="32">
         <f>H43/J43</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L43" s="50"/>
-      <c r="M43" s="50"/>
-      <c r="N43" s="50"/>
+        <v>1953.46456708295</v>
+      </c>
+      <c r="L43" s="48"/>
+      <c r="M43" s="48"/>
+      <c r="N43" s="48"/>
       <c r="P43" s="29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q43" s="29">
         <v>100000</v>
@@ -4450,19 +6473,38 @@
         <v>2</v>
       </c>
       <c r="S43" s="29">
-        <v>34.976300000000002</v>
+        <v>26.713999999999999</v>
       </c>
       <c r="T43" s="32">
         <f>Q43/S43</f>
-        <v>2859.0788619722498</v>
-      </c>
-      <c r="U43" s="50"/>
-      <c r="V43" s="50"/>
-      <c r="W43" s="50"/>
-    </row>
-    <row r="44" spans="7:23" x14ac:dyDescent="0.25">
+        <v>3743.3555439095608</v>
+      </c>
+      <c r="U43" s="48"/>
+      <c r="V43" s="48"/>
+      <c r="W43" s="48"/>
+      <c r="Y43" s="29">
+        <v>3</v>
+      </c>
+      <c r="Z43" s="29">
+        <v>100000</v>
+      </c>
+      <c r="AA43" s="29">
+        <v>3</v>
+      </c>
+      <c r="AB43" s="29">
+        <v>25.487200000000001</v>
+      </c>
+      <c r="AC43" s="32">
+        <f>Z43/AB43</f>
+        <v>3923.5380897077748</v>
+      </c>
+      <c r="AD43" s="2"/>
+      <c r="AE43" s="2"/>
+      <c r="AF43" s="2"/>
+    </row>
+    <row r="44" spans="7:32" x14ac:dyDescent="0.25">
       <c r="G44" s="29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H44" s="29">
         <v>100000</v>
@@ -4470,16 +6512,18 @@
       <c r="I44" s="27">
         <v>1</v>
       </c>
-      <c r="J44" s="29"/>
-      <c r="K44" s="32" t="e">
+      <c r="J44" s="29">
+        <v>45.819600000000001</v>
+      </c>
+      <c r="K44" s="32">
         <f>H44/J44</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L44" s="50"/>
-      <c r="M44" s="50"/>
-      <c r="N44" s="50"/>
+        <v>2182.4721298309018</v>
+      </c>
+      <c r="L44" s="48"/>
+      <c r="M44" s="48"/>
+      <c r="N44" s="48"/>
       <c r="P44" s="29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q44" s="29">
         <v>100000</v>
@@ -4488,19 +6532,38 @@
         <v>2</v>
       </c>
       <c r="S44" s="29">
-        <v>26.713999999999999</v>
+        <v>28.513000000000002</v>
       </c>
       <c r="T44" s="32">
         <f>Q44/S44</f>
-        <v>3743.3555439095608</v>
-      </c>
-      <c r="U44" s="50"/>
-      <c r="V44" s="50"/>
-      <c r="W44" s="50"/>
-    </row>
-    <row r="45" spans="7:23" x14ac:dyDescent="0.25">
+        <v>3507.1721670816819</v>
+      </c>
+      <c r="U44" s="48"/>
+      <c r="V44" s="48"/>
+      <c r="W44" s="48"/>
+      <c r="Y44" s="29">
+        <v>4</v>
+      </c>
+      <c r="Z44" s="29">
+        <v>100000</v>
+      </c>
+      <c r="AA44" s="29">
+        <v>3</v>
+      </c>
+      <c r="AB44" s="29">
+        <v>26.460599999999999</v>
+      </c>
+      <c r="AC44" s="32">
+        <f>Z44/AB44</f>
+        <v>3779.2037973439756</v>
+      </c>
+      <c r="AD44" s="2"/>
+      <c r="AE44" s="2"/>
+      <c r="AF44" s="2"/>
+    </row>
+    <row r="45" spans="7:32" x14ac:dyDescent="0.25">
       <c r="G45" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H45" s="29">
         <v>100000</v>
@@ -4508,16 +6571,18 @@
       <c r="I45" s="27">
         <v>1</v>
       </c>
-      <c r="J45" s="29"/>
-      <c r="K45" s="32" t="e">
+      <c r="J45" s="29">
+        <v>51.723500000000001</v>
+      </c>
+      <c r="K45" s="32">
         <f>H45/J45</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L45" s="50"/>
-      <c r="M45" s="50"/>
-      <c r="N45" s="50"/>
+        <v>1933.3571780718628</v>
+      </c>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="49"/>
       <c r="P45" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q45" s="29">
         <v>100000</v>
@@ -4526,106 +6591,121 @@
         <v>2</v>
       </c>
       <c r="S45" s="29">
-        <v>28.513000000000002</v>
+        <v>26.377700000000001</v>
       </c>
       <c r="T45" s="32">
         <f>Q45/S45</f>
-        <v>3507.1721670816819</v>
-      </c>
-      <c r="U45" s="50"/>
-      <c r="V45" s="50"/>
-      <c r="W45" s="50"/>
-    </row>
-    <row r="46" spans="7:23" x14ac:dyDescent="0.25">
-      <c r="G46" s="29">
+        <v>3791.0811025980279</v>
+      </c>
+      <c r="U45" s="49"/>
+      <c r="V45" s="49"/>
+      <c r="W45" s="49"/>
+      <c r="Y45" s="29">
         <v>5</v>
       </c>
-      <c r="H46" s="29">
+      <c r="Z45" s="29">
         <v>100000</v>
       </c>
-      <c r="I46" s="27">
-        <v>1</v>
-      </c>
-      <c r="J46" s="29"/>
-      <c r="K46" s="32" t="e">
-        <f>H46/J46</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L46" s="51"/>
-      <c r="M46" s="51"/>
-      <c r="N46" s="51"/>
-      <c r="P46" s="29">
-        <v>5</v>
-      </c>
-      <c r="Q46" s="29">
-        <v>100000</v>
-      </c>
-      <c r="R46" s="29">
-        <v>2</v>
-      </c>
-      <c r="S46" s="29">
-        <v>26.377700000000001</v>
-      </c>
-      <c r="T46" s="32">
-        <f>Q46/S46</f>
-        <v>3791.0811025980279</v>
-      </c>
-      <c r="U46" s="51"/>
-      <c r="V46" s="51"/>
-      <c r="W46" s="51"/>
-    </row>
-    <row r="47" spans="7:23" x14ac:dyDescent="0.25">
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="41"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="39"/>
-      <c r="L47" s="41"/>
-      <c r="M47" s="41">
-        <f>MEDIAN(M30,M36,M42)</f>
-        <v>1.3248099143462695</v>
-      </c>
-      <c r="N47" s="41" t="e">
-        <f>AVERAGE(N30,N36,N42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P47" s="41"/>
-      <c r="Q47" s="41"/>
-      <c r="R47" s="41"/>
-      <c r="S47" s="41"/>
-      <c r="T47" s="39"/>
-      <c r="U47" s="41"/>
-      <c r="V47" s="41">
-        <f>MEDIAN(V30,V36,V42)</f>
+      <c r="AA45" s="29">
+        <v>3</v>
+      </c>
+      <c r="AB45" s="29">
+        <v>26.930099999999999</v>
+      </c>
+      <c r="AC45" s="32">
+        <f>Z45/AB45</f>
+        <v>3713.3170690045713</v>
+      </c>
+      <c r="AD45" s="2"/>
+      <c r="AE45" s="2"/>
+      <c r="AF45" s="2"/>
+    </row>
+    <row r="46" spans="7:32" x14ac:dyDescent="0.25">
+      <c r="G46" s="39"/>
+      <c r="H46" s="39"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="39"/>
+      <c r="M46" s="39">
+        <f>MEDIAN(M29,M35,M41)</f>
+        <v>1.2773538825599564</v>
+      </c>
+      <c r="N46" s="39">
+        <f>AVERAGE(N29,N35,N41)</f>
+        <v>5279.7587380201294</v>
+      </c>
+      <c r="P46" s="39"/>
+      <c r="Q46" s="39"/>
+      <c r="R46" s="39"/>
+      <c r="S46" s="39"/>
+      <c r="T46" s="37"/>
+      <c r="U46" s="39"/>
+      <c r="V46" s="39">
+        <f>MEDIAN(V29,V35,V41)</f>
         <v>2.2949191030371843</v>
       </c>
-      <c r="W47" s="41">
-        <f>AVERAGE(W30,W36,W42)</f>
+      <c r="W46" s="39">
+        <f>AVERAGE(W29,W35,W41)</f>
         <v>8567.6938237220256</v>
       </c>
+      <c r="Y46" s="29"/>
+      <c r="Z46" s="29"/>
+      <c r="AA46" s="29"/>
+      <c r="AB46" s="29"/>
+      <c r="AC46" s="32"/>
+      <c r="AD46" s="33"/>
+      <c r="AE46" s="33"/>
+      <c r="AF46" s="33"/>
+    </row>
+    <row r="47" spans="7:32" x14ac:dyDescent="0.25">
+      <c r="Y47" s="39"/>
+      <c r="Z47" s="39"/>
+      <c r="AA47" s="39"/>
+      <c r="AB47" s="39"/>
+      <c r="AC47" s="37"/>
+      <c r="AD47" s="39"/>
+      <c r="AE47" s="39">
+        <f>MEDIAN(AE29,AE35,AE41)</f>
+        <v>2.2276478991406088</v>
+      </c>
+      <c r="AF47" s="39">
+        <f>AVERAGE(AF29,AF35,AF41)</f>
+        <v>8595.885659030946</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="54">
-    <mergeCell ref="U36:U40"/>
-    <mergeCell ref="U42:U46"/>
-    <mergeCell ref="V36:V40"/>
-    <mergeCell ref="V42:V46"/>
-    <mergeCell ref="W36:W40"/>
-    <mergeCell ref="W42:W46"/>
-    <mergeCell ref="G28:L28"/>
-    <mergeCell ref="U30:U34"/>
-    <mergeCell ref="V30:V34"/>
-    <mergeCell ref="W30:W34"/>
-    <mergeCell ref="L30:L34"/>
-    <mergeCell ref="M30:M34"/>
-    <mergeCell ref="L36:L40"/>
-    <mergeCell ref="M36:M40"/>
-    <mergeCell ref="L42:L46"/>
-    <mergeCell ref="M42:M46"/>
-    <mergeCell ref="N42:N46"/>
-    <mergeCell ref="N36:N40"/>
-    <mergeCell ref="N30:N34"/>
-    <mergeCell ref="P28:U28"/>
+  <mergeCells count="64">
+    <mergeCell ref="AD41:AD45"/>
+    <mergeCell ref="AE41:AE45"/>
+    <mergeCell ref="AF41:AF45"/>
+    <mergeCell ref="Y27:AD27"/>
+    <mergeCell ref="AD29:AD33"/>
+    <mergeCell ref="AE29:AE33"/>
+    <mergeCell ref="AF29:AF33"/>
+    <mergeCell ref="AD35:AD39"/>
+    <mergeCell ref="AE35:AE39"/>
+    <mergeCell ref="AF35:AF39"/>
+    <mergeCell ref="U35:U39"/>
+    <mergeCell ref="U41:U45"/>
+    <mergeCell ref="V35:V39"/>
+    <mergeCell ref="V41:V45"/>
+    <mergeCell ref="W35:W39"/>
+    <mergeCell ref="W41:W45"/>
+    <mergeCell ref="G27:L27"/>
+    <mergeCell ref="U29:U33"/>
+    <mergeCell ref="V29:V33"/>
+    <mergeCell ref="W29:W33"/>
+    <mergeCell ref="L29:L33"/>
+    <mergeCell ref="M29:M33"/>
+    <mergeCell ref="L35:L39"/>
+    <mergeCell ref="M35:M39"/>
+    <mergeCell ref="L41:L45"/>
+    <mergeCell ref="M41:M45"/>
+    <mergeCell ref="N41:N45"/>
+    <mergeCell ref="N35:N39"/>
+    <mergeCell ref="N29:N33"/>
+    <mergeCell ref="P27:U27"/>
     <mergeCell ref="V15:V19"/>
     <mergeCell ref="W15:W19"/>
     <mergeCell ref="AD15:AD19"/>
@@ -4662,16 +6742,16 @@
     <mergeCell ref="AD3:AD7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:E21"/>
+  <dimension ref="B2:Y31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4682,7 +6762,9 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C2" s="14"/>
+      <c r="C2" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C3" s="14" t="s">
@@ -4692,19 +6774,19 @@
         <v>13</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="42">
-        <f>'v1 (lote de 50)'!M21</f>
+      <c r="D4" s="40">
+        <f>'v1 (lote de 50)'!M20</f>
         <v>0.76684661340243288</v>
       </c>
-      <c r="E4" s="42">
-        <f>'v1 (lote de 50)'!N21</f>
+      <c r="E4" s="40">
+        <f>'v1 (lote de 50)'!N20</f>
         <v>2801.2535394421488</v>
       </c>
     </row>
@@ -4712,12 +6794,12 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="42">
-        <f>'v1 (lote de 50)'!V21</f>
+      <c r="D5" s="40">
+        <f>'v1 (lote de 50)'!V20</f>
         <v>1.2350227209496429</v>
       </c>
-      <c r="E5" s="42">
-        <f>'v1 (lote de 50)'!W21</f>
+      <c r="E5" s="40">
+        <f>'v1 (lote de 50)'!W20</f>
         <v>4649.4029294504235</v>
       </c>
     </row>
@@ -4725,39 +6807,97 @@
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6" s="42">
-        <f>'v1 (lote de 50)'!AE21</f>
+      <c r="D6" s="40">
+        <f>'v1 (lote de 50)'!AE20</f>
         <v>1.5533490799871694</v>
       </c>
-      <c r="E6" s="42">
-        <f>'v1 (lote de 50)'!AF21</f>
-        <v>5434.9836444001312</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="40">
+        <f>'v1 (lote de 50)'!AF20</f>
+        <v>5778.0613592740383</v>
+      </c>
+    </row>
+    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="Y18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>23</v>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="40">
+        <f>'v1 (lote de 50)'!M46</f>
+        <v>1.2773538825599564</v>
+      </c>
+      <c r="E29" s="40">
+        <f>'v1 (lote de 50)'!N46</f>
+        <v>5279.7587380201294</v>
+      </c>
+    </row>
+    <row r="30" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" s="40">
+        <f>'v1 (lote de 50)'!V46</f>
+        <v>2.2949191030371843</v>
+      </c>
+      <c r="E30" s="40">
+        <f>'v1 (lote de 50)'!W46</f>
+        <v>8567.6938237220256</v>
+      </c>
+    </row>
+    <row r="31" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31" s="40">
+        <f>'v1 (lote de 50)'!AE47</f>
+        <v>2.2276478991406088</v>
+      </c>
+      <c r="E31" s="40">
+        <f>'v1 (lote de 50)'!AF47</f>
+        <v>8595.885659030946</v>
       </c>
     </row>
   </sheetData>

</xml_diff>